<commit_message>
ask user for the name of the product
</commit_message>
<xml_diff>
--- a/dados/lista_urls.xlsx
+++ b/dados/lista_urls.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A217"/>
+  <dimension ref="A1:A222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1940,6 +1940,41 @@
         </is>
       </c>
     </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/apple-iphone-14-128-gb-amarelo-distribuidor-autorizado/p/MLB1024156591?pdp_filters=category:MLB1055#searchVariation=MLB1024156591&amp;position=2&amp;search_layout=stack&amp;type=product&amp;tracking_id=c9fc395a-5c68-4423-a1b3-0cf8f16d183f</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/apple-iphone-13-128-gb-estelar-distribuidor-autorizado/p/MLB1018500855?pdp_filters=category:MLB1055#searchVariation=MLB1018500855&amp;position=3&amp;search_layout=stack&amp;type=product&amp;tracking_id=c9fc395a-5c68-4423-a1b3-0cf8f16d183f</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/apple-iphone-14-128-gb-meia-noite-distribuidor-autorizado/p/MLB1019615360?pdp_filters=category:MLB1055#searchVariation=MLB1019615360&amp;position=4&amp;search_layout=stack&amp;type=product&amp;tracking_id=c9fc395a-5c68-4423-a1b3-0cf8f16d183f</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/apple-iphone-13-128-gb-meia-noite-distribuidor-autorizado/p/MLB1018500844?pdp_filters=category:MLB1055#searchVariation=MLB1018500844&amp;position=5&amp;search_layout=stack&amp;type=product&amp;tracking_id=c9fc395a-5c68-4423-a1b3-0cf8f16d183f</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/apple-iphone-14-128-gb-estelar-distribuidor-autorizado/p/MLB1019615378?pdp_filters=category:MLB1055#searchVariation=MLB1019615378&amp;position=6&amp;search_layout=stack&amp;type=product&amp;tracking_id=c9fc395a-5c68-4423-a1b3-0cf8f16d183f</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
recuperação da informação e ranking
</commit_message>
<xml_diff>
--- a/dados/lista_urls.xlsx
+++ b/dados/lista_urls.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A442"/>
+  <dimension ref="A1:A462"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3515,6 +3515,146 @@
         </is>
       </c>
     </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/kit-canetas-gel-48-cores-glitter-metalico-pastel-e-neon-exterior-preto/p/MLB24557984#searchVariation=MLB24557984&amp;position=2&amp;search_layout=grid&amp;type=product&amp;tracking_id=99ea6a2f-141a-4527-8f23-eb37cfbe5738</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/15-canetas-fofas-variadas-atacado-papelaria-escolar-tinta-preto/p/MLB35822093#searchVariation=MLB35822093&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=99ea6a2f-141a-4527-8f23-eb37cfbe5738</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-esferografica-compactor-caixa-com-100-unidades-cor-da-tinta-azul-cor-do-exterior-cristal/p/MLB22766681#searchVariation=MLB22766681&amp;position=4&amp;search_layout=grid&amp;type=product&amp;tracking_id=99ea6a2f-141a-4527-8f23-eb37cfbe5738</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-bic-cristal-preciso-08mm-azul-caixa-c-50-cor-do-exterior-transparente/p/MLB22706525#searchVariation=MLB22706525&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=99ea6a2f-141a-4527-8f23-eb37cfbe5738</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/marcador-retroprojetor-cd-20mm-jocar-preta-cx12/p/MLB24732135#searchVariation=MLB24732135&amp;position=8&amp;search_layout=grid&amp;type=product&amp;tracking_id=99ea6a2f-141a-4527-8f23-eb37cfbe5738</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/kit-canetas-gel-48-cores-glitter-metalico-pastel-e-neon-exterior-preto/p/MLB24557984#searchVariation=MLB24557984&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=f388956c-6f7b-4731-9720-0a2a59b89c52</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/15-canetas-fofas-variadas-atacado-papelaria-escolar-tinta-preto/p/MLB35822093#searchVariation=MLB35822093&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=f388956c-6f7b-4731-9720-0a2a59b89c52</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-esferografica-compactor-caixa-com-100-unidades-cor-da-tinta-azul-cor-do-exterior-cristal/p/MLB22766681#searchVariation=MLB22766681&amp;position=13&amp;search_layout=grid&amp;type=product&amp;tracking_id=f388956c-6f7b-4731-9720-0a2a59b89c52</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-bic-cristal-preciso-08mm-azul-caixa-c-50-cor-do-exterior-transparente/p/MLB22706525#searchVariation=MLB22706525&amp;position=18&amp;search_layout=grid&amp;type=product&amp;tracking_id=f388956c-6f7b-4731-9720-0a2a59b89c52</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/marcador-retroprojetor-cd-20mm-jocar-preta-cx12/p/MLB24732135#searchVariation=MLB24732135&amp;position=17&amp;search_layout=grid&amp;type=product&amp;tracking_id=f388956c-6f7b-4731-9720-0a2a59b89c52</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/kit-canetas-gel-48-cores-glitter-metalico-pastel-e-neon-exterior-preto/p/MLB24557984#searchVariation=MLB24557984&amp;position=2&amp;search_layout=grid&amp;type=product&amp;tracking_id=aa23c399-e12c-417b-a8a6-453afd5fbb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/15-canetas-fofas-variadas-atacado-papelaria-escolar-tinta-preto/p/MLB35822093#searchVariation=MLB35822093&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=aa23c399-e12c-417b-a8a6-453afd5fbb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-esferografica-compactor-caixa-com-100-unidades-cor-da-tinta-azul-cor-do-exterior-cristal/p/MLB22766681#searchVariation=MLB22766681&amp;position=4&amp;search_layout=grid&amp;type=product&amp;tracking_id=aa23c399-e12c-417b-a8a6-453afd5fbb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-bic-cristal-preciso-08mm-azul-caixa-c-50-cor-do-exterior-transparente/p/MLB22706525#searchVariation=MLB22706525&amp;position=5&amp;search_layout=grid&amp;type=product&amp;tracking_id=aa23c399-e12c-417b-a8a6-453afd5fbb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/marcador-retroprojetor-cd-20mm-jocar-preta-cx12/p/MLB24732135#searchVariation=MLB24732135&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=aa23c399-e12c-417b-a8a6-453afd5fbb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/kit-canetas-gel-48-cores-glitter-metalico-pastel-e-neon-exterior-preto/p/MLB24557984#searchVariation=MLB24557984&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=98004e2a-881f-4d7a-8410-df5355e4ccf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/15-canetas-fofas-variadas-atacado-papelaria-escolar-tinta-preto/p/MLB35822093#searchVariation=MLB35822093&amp;position=5&amp;search_layout=grid&amp;type=product&amp;tracking_id=98004e2a-881f-4d7a-8410-df5355e4ccf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-esferografica-compactor-caixa-com-100-unidades-cor-da-tinta-azul-cor-do-exterior-cristal/p/MLB22766681#searchVariation=MLB22766681&amp;position=7&amp;search_layout=grid&amp;type=product&amp;tracking_id=98004e2a-881f-4d7a-8410-df5355e4ccf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/caneta-bic-cristal-preciso-08mm-azul-caixa-c-50-cor-do-exterior-transparente/p/MLB22706525#searchVariation=MLB22706525&amp;position=9&amp;search_layout=grid&amp;type=product&amp;tracking_id=98004e2a-881f-4d7a-8410-df5355e4ccf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/marcador-retroprojetor-cd-20mm-jocar-preta-cx12/p/MLB24732135#searchVariation=MLB24732135&amp;position=17&amp;search_layout=grid&amp;type=product&amp;tracking_id=98004e2a-881f-4d7a-8410-df5355e4ccf9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>